<commit_message>
cleaner code with synonym search
</commit_message>
<xml_diff>
--- a/UniversityPrograms.xlsx
+++ b/UniversityPrograms.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Venu\python\workspace\git\chatbot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Venu\python\workspace\test2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7DD137-16A1-4C24-8B91-DC8FF23A63E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721FB959-7402-42C1-9F1C-D1EF16F1EA22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="university" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>University</t>
-  </si>
-  <si>
     <t>HIGHER EDUCATION ACADEMY</t>
   </si>
   <si>
@@ -46,6 +43,9 @@
   </si>
   <si>
     <t>UNIVERSITY OF PORTSMOUTH</t>
+  </si>
+  <si>
+    <t>university</t>
   </si>
 </sst>
 </file>
@@ -366,7 +366,7 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -376,37 +376,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>